<commit_message>
(feature/sdbDetails): fix importexcel break loop; add claim login, authorize role in controller
</commit_message>
<xml_diff>
--- a/server/Uploads/academicyear.xlsx
+++ b/server/Uploads/academicyear.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenhu\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenhu\OneDrive\Máy tính\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DFFC4E1-1E76-42B5-BC85-CFB89A6D06C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2E58255-5699-4448-BAFA-09B66AD3BCF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{89160CE7-9443-4C42-AF38-5D727278BB7D}"/>
   </bookViews>
@@ -462,7 +462,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E12"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>